<commit_message>
deshmia dhe situacioni permirsim i nr parceles
</commit_message>
<xml_diff>
--- a/1-Situacioni/regjistri/Koordinatat.xlsx
+++ b/1-Situacioni/regjistri/Koordinatat.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="8">
   <si>
     <t>Shtëpi-Ndërtesë</t>
   </si>
@@ -46,20 +46,17 @@
     <t>Përshkrimi</t>
   </si>
   <si>
-    <t>Koordinatat e parceles 734-18</t>
-  </si>
-  <si>
-    <t>Koordinatat e parceles 733-20</t>
+    <t>Koordinatat e parceles 3227-0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,7 +248,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -283,9 +280,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -317,6 +315,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -492,14 +491,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="3.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -513,7 +512,7 @@
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
@@ -538,7 +537,7 @@
       <c r="J2" s="7"/>
       <c r="K2" s="8"/>
     </row>
-    <row r="3" spans="2:11">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="3">
         <v>12</v>
       </c>
@@ -567,7 +566,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:11">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
         <v>13</v>
       </c>
@@ -596,7 +595,7 @@
         <v>4692127.443</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="15" customHeight="1">
+    <row r="5" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>15</v>
       </c>
@@ -616,16 +615,16 @@
         <v>0</v>
       </c>
       <c r="I5" s="3">
-        <v>181505</v>
+        <v>168622</v>
       </c>
       <c r="J5" s="4">
-        <v>7511887.4450000003</v>
+        <v>7511867.7390000001</v>
       </c>
       <c r="K5" s="4">
-        <v>4692119.66</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" ht="15" customHeight="1">
+        <v>4692128.4790000003</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <v>16</v>
       </c>
@@ -645,16 +644,16 @@
         <v>0</v>
       </c>
       <c r="I6" s="3">
-        <v>181506</v>
+        <v>181505</v>
       </c>
       <c r="J6" s="4">
-        <v>7511888.2970000003</v>
+        <v>7511887.4450000003</v>
       </c>
       <c r="K6" s="4">
-        <v>4692127.3020000001</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" ht="15" customHeight="1">
+        <v>4692119.66</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
         <v>17</v>
       </c>
@@ -674,16 +673,16 @@
         <v>0</v>
       </c>
       <c r="I7" s="3">
-        <v>182180</v>
+        <v>181506</v>
       </c>
       <c r="J7" s="4">
-        <v>7511884.9419999998</v>
+        <v>7511888.2970000003</v>
       </c>
       <c r="K7" s="4">
-        <v>4692123.3310000002</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" ht="15" customHeight="1">
+        <v>4692127.3020000001</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
         <v>18</v>
       </c>
@@ -702,8 +701,17 @@
       <c r="G8" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="2:11" ht="15" customHeight="1">
+      <c r="I8" s="3">
+        <v>181509</v>
+      </c>
+      <c r="J8" s="4">
+        <v>7511886.7010000004</v>
+      </c>
+      <c r="K8" s="4">
+        <v>4692113</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
         <v>19</v>
       </c>
@@ -722,13 +730,17 @@
       <c r="G9" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="J9" s="7"/>
-      <c r="K9" s="8"/>
-    </row>
-    <row r="10" spans="2:11" ht="15" customHeight="1">
+      <c r="I9" s="3">
+        <v>182181</v>
+      </c>
+      <c r="J9" s="4">
+        <v>7511866.2699999996</v>
+      </c>
+      <c r="K9" s="4">
+        <v>4692115.7300000004</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>20</v>
       </c>
@@ -747,17 +759,8 @@
       <c r="G10" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I10" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" ht="15" customHeight="1">
+    </row>
+    <row r="11" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <v>25</v>
       </c>
@@ -776,17 +779,8 @@
       <c r="G11" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I11" s="3">
-        <v>168621</v>
-      </c>
-      <c r="J11" s="4">
-        <v>7511885.8310000002</v>
-      </c>
-      <c r="K11" s="4">
-        <v>4692127.443</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" ht="15" customHeight="1">
+    </row>
+    <row r="12" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <v>27</v>
       </c>
@@ -805,17 +799,8 @@
       <c r="G12" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I12" s="3">
-        <v>168622</v>
-      </c>
-      <c r="J12" s="4">
-        <v>7511867.7390000001</v>
-      </c>
-      <c r="K12" s="4">
-        <v>4692128.4790000003</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" ht="15" customHeight="1">
+    </row>
+    <row r="13" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <v>55</v>
       </c>
@@ -834,17 +819,8 @@
       <c r="G13" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I13" s="3">
-        <v>181505</v>
-      </c>
-      <c r="J13" s="4">
-        <v>7511887.4450000003</v>
-      </c>
-      <c r="K13" s="4">
-        <v>4692119.66</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" ht="15" customHeight="1">
+    </row>
+    <row r="14" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <v>56</v>
       </c>
@@ -863,17 +839,8 @@
       <c r="G14" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I14" s="3">
-        <v>181509</v>
-      </c>
-      <c r="J14" s="4">
-        <v>7511886.7010000004</v>
-      </c>
-      <c r="K14" s="4">
-        <v>4692113</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11">
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <v>57</v>
       </c>
@@ -892,68 +859,50 @@
       <c r="G15" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I15" s="3">
-        <v>182180</v>
-      </c>
-      <c r="J15" s="4">
-        <v>7511884.9419999998</v>
-      </c>
-      <c r="K15" s="4">
-        <v>4692123.3310000002</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11">
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16"/>
       <c r="E16"/>
       <c r="F16"/>
-      <c r="I16" s="3">
-        <v>182181</v>
-      </c>
-      <c r="J16" s="4">
-        <v>7511866.2699999996</v>
-      </c>
-      <c r="K16" s="4">
-        <v>4692115.7300000004</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7">
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17"/>
       <c r="C17"/>
       <c r="D17"/>
       <c r="E17"/>
       <c r="F17"/>
     </row>
-    <row r="18" spans="2:7">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18"/>
       <c r="C18"/>
       <c r="D18"/>
       <c r="E18"/>
       <c r="F18"/>
     </row>
-    <row r="19" spans="2:7">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19"/>
       <c r="C19"/>
       <c r="D19"/>
       <c r="E19"/>
       <c r="F19"/>
     </row>
-    <row r="20" spans="2:7">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20"/>
       <c r="C20"/>
       <c r="D20"/>
       <c r="E20"/>
       <c r="F20"/>
     </row>
-    <row r="21" spans="2:7">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21"/>
       <c r="C21"/>
       <c r="D21"/>
       <c r="E21"/>
       <c r="F21"/>
     </row>
-    <row r="22" spans="2:7">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22"/>
       <c r="C22"/>
       <c r="D22"/>
@@ -961,49 +910,49 @@
       <c r="F22"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="2:7">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23"/>
       <c r="C23"/>
       <c r="D23"/>
       <c r="E23"/>
       <c r="F23"/>
     </row>
-    <row r="24" spans="2:7">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24"/>
       <c r="C24"/>
       <c r="D24"/>
       <c r="E24"/>
       <c r="F24"/>
     </row>
-    <row r="25" spans="2:7">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25"/>
       <c r="C25"/>
       <c r="D25"/>
       <c r="E25"/>
       <c r="F25"/>
     </row>
-    <row r="26" spans="2:7">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26"/>
       <c r="C26"/>
       <c r="D26"/>
       <c r="E26"/>
       <c r="F26"/>
     </row>
-    <row r="27" spans="2:7">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27"/>
       <c r="C27"/>
       <c r="D27"/>
       <c r="E27"/>
       <c r="F27"/>
     </row>
-    <row r="28" spans="2:7">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28"/>
       <c r="C28"/>
       <c r="D28"/>
       <c r="E28"/>
       <c r="F28"/>
     </row>
-    <row r="29" spans="2:7">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29"/>
       <c r="C29"/>
       <c r="D29"/>
@@ -1011,9 +960,8 @@
       <c r="F29"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="I2:K2"/>
-    <mergeCell ref="I9:K9"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1022,14 +970,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="5" width="16.5703125" customWidth="1"/>
   </cols>
@@ -1040,12 +988,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>